<commit_message>
For Demo to Sudar
</commit_message>
<xml_diff>
--- a/data/RS_CampaignE2E.xlsx
+++ b/data/RS_CampaignE2E.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr documentId="13_ncr:1_{DE51C39F-DAB8-4D72-A730-8D7E9E94F865}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34"/>
+  <xr:revisionPtr documentId="13_ncr:1_{5EBFDF7E-DF86-4A2F-BDF9-76EE32E7F4F3}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34"/>
   <bookViews>
     <workbookView activeTab="1" tabRatio="639" windowHeight="12645" windowWidth="22260" xWindow="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="0"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="120">
   <si>
     <t>campTypeIndex</t>
   </si>
@@ -379,14 +379,18 @@
     <t>Sender: Reg_Test Brand ENG</t>
   </si>
   <si>
-    <t>Subject: Reg_Test Brand ENG</t>
-  </si>
-  <si>
-    <t>Banner: Reg_Test Brand ENG</t>
-  </si>
-  <si>
     <t>Hello (FirstName) (LastName)
 Reg_Test Brand ENG</t>
+  </si>
+  <si>
+    <t>Subject: Reg_Test Brand ENG (FirstName) (LastName)</t>
+  </si>
+  <si>
+    <t>Banner: Reg_Test Brand ENG (FirstName) (LastName)</t>
+  </si>
+  <si>
+    <t>Thank you
+(FirstName) (LastName)</t>
   </si>
 </sst>
 </file>
@@ -1056,8 +1060,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0200146-B3F6-478E-BE48-14E6C2EC7AB7}">
   <dimension ref="A1:Q35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E19" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+    <sheetView tabSelected="1" topLeftCell="E13" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1260,7 +1264,7 @@
         <v>29</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="K15" s="4" t="s">
         <v>83</v>
@@ -1271,7 +1275,7 @@
         <v>9</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="K16" s="4" t="s">
         <v>84</v>
@@ -1291,18 +1295,18 @@
         <v>10</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="K18" s="4" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row ht="30" r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>54</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>43</v>
+        <v>119</v>
       </c>
       <c r="K19" s="4" t="s">
         <v>43</v>

</xml_diff>

<commit_message>
made changes for versions and added change to create test evidence using the method addEvidence()
</commit_message>
<xml_diff>
--- a/data/RS_CampaignE2E.xlsx
+++ b/data/RS_CampaignE2E.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr documentId="13_ncr:1_{7F593AE8-1920-40D4-BA9D-EABCFCF809F5}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34"/>
+  <xr:revisionPtr documentId="13_ncr:1_{7944B36B-7FA7-402B-9F52-F5FD9BA03BB9}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40"/>
   <bookViews>
     <workbookView tabRatio="639" windowHeight="12645" windowWidth="22260" xWindow="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="0"/>
   </bookViews>
@@ -368,9 +368,6 @@
 (FirstName) (LastName)</t>
   </si>
   <si>
-    <t>DF - German</t>
-  </si>
-  <si>
     <t>Reg_Test Loc ENG</t>
   </si>
   <si>
@@ -390,6 +387,9 @@
   </si>
   <si>
     <t>Banner: Reg_Test MLC ENG (FirstName) (LastName)</t>
+  </si>
+  <si>
+    <t>DF</t>
   </si>
 </sst>
 </file>
@@ -743,8 +743,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView tabSelected="1" topLeftCell="B8" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -863,7 +863,7 @@
         <v>3</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K7" s="4" t="s">
         <v>78</v>
@@ -874,7 +874,7 @@
         <v>74</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="K8" s="4" t="s">
         <v>75</v>
@@ -885,7 +885,7 @@
         <v>5</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K9" s="4" t="s">
         <v>79</v>
@@ -896,7 +896,7 @@
         <v>6</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K10" s="4" t="s">
         <v>80</v>
@@ -949,7 +949,7 @@
         <v>29</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K15" s="4" t="s">
         <v>47</v>
@@ -960,7 +960,7 @@
         <v>9</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K16" s="4" t="s">
         <v>48</v>
@@ -1626,7 +1626,7 @@
         <v>29</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row ht="30" r="16" spans="1:16" x14ac:dyDescent="0.25">
@@ -1634,7 +1634,7 @@
         <v>9</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row customHeight="1" ht="190.5" r="17" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>